<commit_message>
Update CI5 ASR CR specific with str.strip() for space to be removed
</commit_message>
<xml_diff>
--- a/data/CI5_ASR_CR_specific_countries.xlsx
+++ b/data/CI5_ASR_CR_specific_countries.xlsx
@@ -46,382 +46,382 @@
     <t>Female</t>
   </si>
   <si>
-    <t xml:space="preserve">Lip                                                                             </t>
+    <t>Lip</t>
   </si>
   <si>
-    <t xml:space="preserve">Tongue                                                                          </t>
+    <t>Tongue</t>
   </si>
   <si>
-    <t xml:space="preserve">Mouth                                                                           </t>
+    <t>Mouth</t>
   </si>
   <si>
-    <t xml:space="preserve">Salivary glands                                                                 </t>
+    <t>Salivary glands</t>
   </si>
   <si>
-    <t xml:space="preserve">Tonsil                                                                          </t>
+    <t>Tonsil</t>
   </si>
   <si>
-    <t xml:space="preserve">Other oropharynx                                                                </t>
+    <t>Other oropharynx</t>
   </si>
   <si>
-    <t xml:space="preserve">Nasopharynx                                                                     </t>
+    <t>Nasopharynx</t>
   </si>
   <si>
-    <t xml:space="preserve">Hypopharynx                                                                     </t>
+    <t>Hypopharynx</t>
   </si>
   <si>
-    <t xml:space="preserve">Pharynx unspecified                                                             </t>
+    <t>Pharynx unspecified</t>
   </si>
   <si>
-    <t xml:space="preserve">Oesophagus                                                                      </t>
+    <t>Oesophagus</t>
   </si>
   <si>
-    <t xml:space="preserve">Stomach                                                                         </t>
+    <t>Stomach</t>
   </si>
   <si>
-    <t xml:space="preserve">Small intestine                                                                 </t>
+    <t>Small intestine</t>
   </si>
   <si>
-    <t xml:space="preserve">Colon                                                                           </t>
+    <t>Colon</t>
   </si>
   <si>
-    <t xml:space="preserve">Rectum                                                                          </t>
+    <t>Rectum</t>
   </si>
   <si>
-    <t xml:space="preserve">Anus                                                                            </t>
+    <t>Anus</t>
   </si>
   <si>
-    <t xml:space="preserve">Liver                                                                           </t>
+    <t>Liver</t>
   </si>
   <si>
-    <t xml:space="preserve">Gallbladder etc.                                                                </t>
+    <t>Gallbladder etc.</t>
   </si>
   <si>
-    <t xml:space="preserve">Pancreas                                                                        </t>
+    <t>Pancreas</t>
   </si>
   <si>
-    <t xml:space="preserve">Nose, sinuses etc.                                                              </t>
+    <t>Nose, sinuses etc.</t>
   </si>
   <si>
-    <t xml:space="preserve">Larynx                                                                          </t>
+    <t>Larynx</t>
   </si>
   <si>
-    <t xml:space="preserve">Lung (incl. trachea and bronchus)                                               </t>
+    <t>Lung (incl. trachea and bronchus)</t>
   </si>
   <si>
-    <t xml:space="preserve">Other thoracic organs                                                           </t>
+    <t>Other thoracic organs</t>
   </si>
   <si>
-    <t xml:space="preserve">Bone                                                                            </t>
+    <t>Bone</t>
   </si>
   <si>
-    <t xml:space="preserve">Melanoma of skin                                                                </t>
+    <t>Melanoma of skin</t>
   </si>
   <si>
-    <t xml:space="preserve">Other skin                                                                      </t>
+    <t>Other skin</t>
   </si>
   <si>
-    <t xml:space="preserve">Mesothelioma                                                                    </t>
+    <t>Mesothelioma</t>
   </si>
   <si>
-    <t xml:space="preserve">Kaposi sarcoma                                                                  </t>
+    <t>Kaposi sarcoma</t>
   </si>
   <si>
-    <t xml:space="preserve">Connective and soft tissue                                                      </t>
+    <t>Connective and soft tissue</t>
   </si>
   <si>
-    <t xml:space="preserve">Breast                                                                          </t>
+    <t>Breast</t>
   </si>
   <si>
-    <t xml:space="preserve">Vulva                                                                           </t>
+    <t>Vulva</t>
   </si>
   <si>
-    <t xml:space="preserve">Vagina                                                                          </t>
+    <t>Vagina</t>
   </si>
   <si>
-    <t xml:space="preserve">Cervix uteri                                                                    </t>
+    <t>Cervix uteri</t>
   </si>
   <si>
-    <t xml:space="preserve">Corpus uteri                                                                    </t>
+    <t>Corpus uteri</t>
   </si>
   <si>
-    <t xml:space="preserve">Uterus unspecified                                                              </t>
+    <t>Uterus unspecified</t>
   </si>
   <si>
-    <t xml:space="preserve">Ovary                                                                           </t>
+    <t>Ovary</t>
   </si>
   <si>
-    <t xml:space="preserve">Other female genital organs                                                     </t>
+    <t>Other female genital organs</t>
   </si>
   <si>
-    <t xml:space="preserve">Placenta                                                                        </t>
+    <t>Placenta</t>
   </si>
   <si>
-    <t xml:space="preserve">Penis                                                                           </t>
+    <t>Penis</t>
   </si>
   <si>
-    <t xml:space="preserve">Prostate                                                                        </t>
+    <t>Prostate</t>
   </si>
   <si>
-    <t xml:space="preserve">Testis                                                                          </t>
+    <t>Testis</t>
   </si>
   <si>
-    <t xml:space="preserve">Other male genital organs                                                       </t>
+    <t>Other male genital organs</t>
   </si>
   <si>
-    <t xml:space="preserve">Kidney                                                                          </t>
+    <t>Kidney</t>
   </si>
   <si>
-    <t xml:space="preserve">Renal pelvis                                                                    </t>
+    <t>Renal pelvis</t>
   </si>
   <si>
-    <t xml:space="preserve">Ureter                                                                          </t>
+    <t>Ureter</t>
   </si>
   <si>
-    <t xml:space="preserve">Bladder                                                                         </t>
+    <t>Bladder</t>
   </si>
   <si>
-    <t xml:space="preserve">Other urinary organs                                                            </t>
+    <t>Other urinary organs</t>
   </si>
   <si>
-    <t xml:space="preserve">Eye                                                                             </t>
+    <t>Eye</t>
   </si>
   <si>
-    <t xml:space="preserve">Brain, nervous system                                                           </t>
+    <t>Brain, nervous system</t>
   </si>
   <si>
-    <t xml:space="preserve">Thyroid                                                                         </t>
+    <t>Thyroid</t>
   </si>
   <si>
-    <t xml:space="preserve">Adrenal gland                                                                   </t>
+    <t>Adrenal gland</t>
   </si>
   <si>
-    <t xml:space="preserve">Other endocrine                                                                 </t>
+    <t>Other endocrine</t>
   </si>
   <si>
-    <t xml:space="preserve">Hodgkin disease                                                                 </t>
+    <t>Hodgkin disease</t>
   </si>
   <si>
-    <t xml:space="preserve">Non-Hodgkin lymphoma                                                            </t>
+    <t>Non-Hodgkin lymphoma</t>
   </si>
   <si>
-    <t xml:space="preserve">Immunoproliferative diseases                                                    </t>
+    <t>Immunoproliferative diseases</t>
   </si>
   <si>
-    <t xml:space="preserve">Multiple myeloma                                                                </t>
+    <t>Multiple myeloma</t>
   </si>
   <si>
-    <t xml:space="preserve">Lymphoid leukaemia                                                              </t>
+    <t>Lymphoid leukaemia</t>
   </si>
   <si>
-    <t xml:space="preserve">Myeloid leukaemia                                                               </t>
+    <t>Myeloid leukaemia</t>
   </si>
   <si>
-    <t xml:space="preserve">Leukaemia unspecified                                                           </t>
+    <t>Leukaemia unspecified</t>
   </si>
   <si>
-    <t xml:space="preserve">Myeloproliferative disorders                                                    </t>
+    <t>Myeloproliferative disorders</t>
   </si>
   <si>
-    <t xml:space="preserve">Myelodysplastic syndromes                                                       </t>
+    <t>Myelodysplastic syndromes</t>
   </si>
   <si>
-    <t xml:space="preserve">Other and unspecified                                                           </t>
+    <t>Other and unspecified</t>
   </si>
   <si>
-    <t xml:space="preserve">All sites                                                                       </t>
+    <t>All sites</t>
   </si>
   <si>
-    <t xml:space="preserve">All sites but skin                                                              </t>
+    <t>All sites but skin</t>
   </si>
   <si>
-    <t xml:space="preserve">C00             </t>
+    <t>C00</t>
   </si>
   <si>
-    <t xml:space="preserve">C01-02          </t>
+    <t>C01-02</t>
   </si>
   <si>
-    <t xml:space="preserve">C03-06          </t>
+    <t>C03-06</t>
   </si>
   <si>
-    <t xml:space="preserve">C07-08          </t>
+    <t>C07-08</t>
   </si>
   <si>
-    <t xml:space="preserve">C09             </t>
+    <t>C09</t>
   </si>
   <si>
-    <t xml:space="preserve">C10             </t>
+    <t>C10</t>
   </si>
   <si>
-    <t xml:space="preserve">C11             </t>
+    <t>C11</t>
   </si>
   <si>
-    <t xml:space="preserve">C12-13          </t>
+    <t>C12-13</t>
   </si>
   <si>
-    <t xml:space="preserve">C14             </t>
+    <t>C14</t>
   </si>
   <si>
-    <t xml:space="preserve">C15             </t>
+    <t>C15</t>
   </si>
   <si>
-    <t xml:space="preserve">C16             </t>
+    <t>C16</t>
   </si>
   <si>
-    <t xml:space="preserve">C17             </t>
+    <t>C17</t>
   </si>
   <si>
-    <t xml:space="preserve">C18             </t>
+    <t>C18</t>
   </si>
   <si>
-    <t xml:space="preserve">C19-20          </t>
+    <t>C19-20</t>
   </si>
   <si>
-    <t xml:space="preserve">C21             </t>
+    <t>C21</t>
   </si>
   <si>
-    <t xml:space="preserve">C22             </t>
+    <t>C22</t>
   </si>
   <si>
-    <t xml:space="preserve">C23-24          </t>
+    <t>C23-24</t>
   </si>
   <si>
-    <t xml:space="preserve">C25             </t>
+    <t>C25</t>
   </si>
   <si>
-    <t xml:space="preserve">C30-31          </t>
+    <t>C30-31</t>
   </si>
   <si>
-    <t xml:space="preserve">C32             </t>
+    <t>C32</t>
   </si>
   <si>
-    <t xml:space="preserve">C33-34          </t>
+    <t>C33-34</t>
   </si>
   <si>
-    <t xml:space="preserve">C37-38          </t>
+    <t>C37-38</t>
   </si>
   <si>
-    <t xml:space="preserve">C40-41          </t>
+    <t>C40-41</t>
   </si>
   <si>
-    <t xml:space="preserve">C43             </t>
+    <t>C43</t>
   </si>
   <si>
-    <t xml:space="preserve">C44             </t>
+    <t>C44</t>
   </si>
   <si>
-    <t xml:space="preserve">C45             </t>
+    <t>C45</t>
   </si>
   <si>
-    <t xml:space="preserve">C46             </t>
+    <t>C46</t>
   </si>
   <si>
-    <t xml:space="preserve">C47+C49         </t>
+    <t>C47+C49</t>
   </si>
   <si>
-    <t xml:space="preserve">C50             </t>
+    <t>C50</t>
   </si>
   <si>
-    <t xml:space="preserve">C51             </t>
+    <t>C51</t>
   </si>
   <si>
-    <t xml:space="preserve">C52             </t>
+    <t>C52</t>
   </si>
   <si>
-    <t xml:space="preserve">C53             </t>
+    <t>C53</t>
   </si>
   <si>
-    <t xml:space="preserve">C54             </t>
+    <t>C54</t>
   </si>
   <si>
-    <t xml:space="preserve">C55             </t>
+    <t>C55</t>
   </si>
   <si>
-    <t xml:space="preserve">C56             </t>
+    <t>C56</t>
   </si>
   <si>
-    <t xml:space="preserve">C57             </t>
+    <t>C57</t>
   </si>
   <si>
-    <t xml:space="preserve">C58             </t>
+    <t>C58</t>
   </si>
   <si>
-    <t xml:space="preserve">C60             </t>
+    <t>C60</t>
   </si>
   <si>
-    <t xml:space="preserve">C61             </t>
+    <t>C61</t>
   </si>
   <si>
-    <t xml:space="preserve">C62             </t>
+    <t>C62</t>
   </si>
   <si>
-    <t xml:space="preserve">C63             </t>
+    <t>C63</t>
   </si>
   <si>
-    <t xml:space="preserve">C64             </t>
+    <t>C64</t>
   </si>
   <si>
-    <t xml:space="preserve">C65             </t>
+    <t>C65</t>
   </si>
   <si>
-    <t xml:space="preserve">C66             </t>
+    <t>C66</t>
   </si>
   <si>
-    <t xml:space="preserve">C67             </t>
+    <t>C67</t>
   </si>
   <si>
-    <t xml:space="preserve">C68             </t>
+    <t>C68</t>
   </si>
   <si>
-    <t xml:space="preserve">C69             </t>
+    <t>C69</t>
   </si>
   <si>
-    <t xml:space="preserve">C70-72          </t>
+    <t>C70-72</t>
   </si>
   <si>
-    <t xml:space="preserve">C73             </t>
+    <t>C73</t>
   </si>
   <si>
-    <t xml:space="preserve">C74             </t>
+    <t>C74</t>
   </si>
   <si>
-    <t xml:space="preserve">C75             </t>
+    <t>C75</t>
   </si>
   <si>
-    <t xml:space="preserve">C81             </t>
+    <t>C81</t>
   </si>
   <si>
-    <t xml:space="preserve">C82-86,C96      </t>
+    <t>C82-86,C96</t>
   </si>
   <si>
-    <t xml:space="preserve">C88             </t>
+    <t>C88</t>
   </si>
   <si>
-    <t xml:space="preserve">C90             </t>
+    <t>C90</t>
   </si>
   <si>
-    <t xml:space="preserve">C91             </t>
+    <t>C91</t>
   </si>
   <si>
-    <t xml:space="preserve">C92-94          </t>
+    <t>C92-94</t>
   </si>
   <si>
-    <t xml:space="preserve">C95             </t>
+    <t>C95</t>
   </si>
   <si>
-    <t xml:space="preserve">MPD             </t>
+    <t>MPD</t>
   </si>
   <si>
-    <t xml:space="preserve">MDS             </t>
+    <t>MDS</t>
   </si>
   <si>
-    <t xml:space="preserve">O&amp;U             </t>
+    <t>O&amp;U</t>
   </si>
   <si>
-    <t xml:space="preserve">ALL             </t>
+    <t>ALL</t>
   </si>
   <si>
-    <t xml:space="preserve">ALLbC44         </t>
+    <t>ALLbC44</t>
   </si>
   <si>
     <t>Mauritius</t>

</xml_diff>